<commit_message>
Updated libraries. Added a setup.bat file that will install all the required third party libraries. Reorganized the files.
</commit_message>
<xml_diff>
--- a/data/dataset.xlsx
+++ b/data/dataset.xlsx
@@ -11,6 +11,7 @@
   </sheets>
   <definedNames>
     <definedName name="bbcnepali" localSheetId="0">Sheet1!$A$1:$C$9</definedName>
+    <definedName name="bbcnepali_1" localSheetId="0">Sheet1!$A$11:$C$82</definedName>
   </definedNames>
   <calcPr calcId="122211"/>
 </workbook>
@@ -27,11 +28,20 @@
       </textFields>
     </textPr>
   </connection>
+  <connection id="2" name="bbcnepali1" type="6" refreshedVersion="5" background="1" saveData="1">
+    <textPr codePage="65001" sourceFile="E:\Projects\SentimentAnalysis\SentimentAnalysis\data\bbcnepali.csv" tab="0" comma="1">
+      <textFields count="3">
+        <textField type="text"/>
+        <textField type="text"/>
+        <textField type="text"/>
+      </textFields>
+    </textPr>
+  </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="188">
   <si>
     <t>939524321575391233</t>
   </si>
@@ -97,6 +107,504 @@
   </si>
   <si>
     <t>@bbcnepali @brb1954 हामी हाम्रै लाइनमा हिँड्नुपर्छ</t>
+  </si>
+  <si>
+    <t>939533844285358081</t>
+  </si>
+  <si>
+    <t>939534892479561728</t>
+  </si>
+  <si>
+    <t>@bbcnepali सिन्को नभाच्ने अनि अनपेक्षित रे वा रे वा ।।।।</t>
+  </si>
+  <si>
+    <t>939665592293789696</t>
+  </si>
+  <si>
+    <t>@bbcnepali @brb1954 पपुलर हुनु र फेमस हुनु फरक कुरा हुन ।  डा. बाबुराम भट्टराईले प्रमाणित गरे ।</t>
+  </si>
+  <si>
+    <t>939662389510676481</t>
+  </si>
+  <si>
+    <t>@bbcnepali तपाईको तयाग खेर जादंईन।धन्यवाद।</t>
+  </si>
+  <si>
+    <t>939634924184727552</t>
+  </si>
+  <si>
+    <t>939528412246536193</t>
+  </si>
+  <si>
+    <t>@bbcnepali यी curd bittenricey जे पनि बोल्छन् भन्ने हाम्लाइ लागि राच</t>
+  </si>
+  <si>
+    <t>939526985813856257</t>
+  </si>
+  <si>
+    <t>@bbcnepali सम्पूर्ण नतीजा पछी बामहरू पनी येसो नभनलान भन्ने छैन ।</t>
+  </si>
+  <si>
+    <t>939649072993935360</t>
+  </si>
+  <si>
+    <t>939532650640850944</t>
+  </si>
+  <si>
+    <t>@bbcnepali @BhagirathYogi दाइ अब बाबुराम दाइ को पार्टी प्रवेश गर्दा होला।</t>
+  </si>
+  <si>
+    <t>939531704770764800</t>
+  </si>
+  <si>
+    <t>@bbcnepali @BhagirathYogi ५ वर्षमा एकपटक मोडन खोजेर कहिलेसम्म मोडिएला नेपालको राजनीति ?</t>
+  </si>
+  <si>
+    <t>939514039566307333</t>
+  </si>
+  <si>
+    <t>@bbcnepali एस्तो भित्र भित्र गर्नुभन्दा खुला एमाले -माओबादी संग गरे जिथ्यो होला. अब भित्री सहमति अनुसार एमालेको भोट हामीलाई आएन अनि हरेको भन्दा सिधा कुरा. के घुमाउनु? मोही माग्ने अनि ढुङ्ग्रो लुकाउने पनि असल संस्कार हो र? बरु बाबुराम इमान्दार एस मानेमा. मोही पनि मागे  ढुङ्ग्रो लुकयेनन.</t>
+  </si>
+  <si>
+    <t>939513364748713984</t>
+  </si>
+  <si>
+    <t>@bbcnepali @RabindraMishra जीको राजीतीमा आगमनले मात्रै धेरै मै हु भन्ने नेताहरुको नींद हराम गरीदिएको थीयो, उहाँले जीतेको भए नेपाली राजनीतिमा नयॉं आयामको झण्डा गाडिन्थ्यो ।</t>
+  </si>
+  <si>
+    <t>939510428643684353</t>
+  </si>
+  <si>
+    <t>@bbcnepali चलखेल...... lol</t>
+  </si>
+  <si>
+    <t>939509252422545409</t>
+  </si>
+  <si>
+    <t>@bbcnepali घोषणापत्र का केहि बुंदाहरु सम्बन्धि प्रस्न गर्दा केहि प्रतिक्रिया गर्नु भएन,मतदाताले सभा र भेलाहरु मा प्रस्न राख्दा समय कम छ भन्दै पन्छिनु भयो,मतदातालाइ प्रस्न गर्न पर्याप्त समय दिनु भएन अनि थोरै मार्जिन बाट हार्दा चलखेल भयो भन्दा राम्रो सुनिएन @bibeksheelnp @RabindraMishra</t>
+  </si>
+  <si>
+    <t>939506908255305730</t>
+  </si>
+  <si>
+    <t>@bbcnepali उनको यही अहमले नै हो विवेकशील साझालाई राष्ट्रिय दलको मान्यता पाउनबाट रोकेको । अहमले जिताउदैन बरु आफैलाई जित्यो भने चाहिँ पतन गराउछ ।</t>
+  </si>
+  <si>
+    <t>939506184494579712</t>
+  </si>
+  <si>
+    <t>@bbcnepali अहिले दोषारोपण गर्दा अरु राजनैतिक दल भन्दा के फरक भयो र। कुनै पनि मान्छेलाई दोष दिदा यथेष्ट प्रमाण देखाउनु जरुरी हुन्छ। अझ पनि @RabindraMishra जस्ता नेताहरुले बाहिरै बसेर पनि धेरै गर्न सक्छन्, पुराना परिपार्टीलाइ त्यागेर सकारात्मक सोच सहित अघि बढ्नुस।</t>
+  </si>
+  <si>
+    <t>939504811073978368</t>
+  </si>
+  <si>
+    <t>@bbcnepali भन्ने बेला चाहिँ विवेकसिल रे, चलखेल होला भन्ने सोचेर पहिले नै विवेक पुर्याउनु पर्थेन?</t>
+  </si>
+  <si>
+    <t>939504017146757122</t>
+  </si>
+  <si>
+    <t>@bbcnepali 😂😂</t>
+  </si>
+  <si>
+    <t>939499929235542017</t>
+  </si>
+  <si>
+    <t>939522624622796800</t>
+  </si>
+  <si>
+    <t>@bbcnepali जनताले विश्वास गरेर नपुग्ने ।अरू कसले विश्वास गर्नुपर्ने हाे।नेपाली कांग्रेस संग मिलेर  एमाले र माअाेवादीले सरकार चलाई सकेकाे हाेईन र। अनि  माअाेवादी र एमाले मिलेर पनि सरकार चलायकै हाे।अधिनायकवाद अाउनेभए त पहिलेनै अाईसकेकाे हुन्थ्यो ।</t>
+  </si>
+  <si>
+    <t>939505773268295680</t>
+  </si>
+  <si>
+    <t>@bbcnepali एकदम ठिक हो ! पुराना प्रतिबद्धता र अनगिन्ती चुनौतीका साथै एत्ति सानो देश र एत्ति जाबो जनताहरुलाइ सुख सुबिधा युक्त बनाइ आत्मनिर्भर बन्ने वातावरण बनाउन सम्पुर्ण सामानहरु आफ्नै देशमा बनाउने र गर्भमा रहेका खनिजहरु उत्खनन गरि देशलाइ बिश्वकै नमूना देश बनाय मात्रै जनताले स्वागत गर्नेछन!</t>
+  </si>
+  <si>
+    <t>939503040763015169</t>
+  </si>
+  <si>
+    <t>@bbcnepali  दुई गोरु मिलेर एउटा गोरुलाई बल मिचाइ भएको छ ।जोत्नको लागि त हलगोरु ठिकै हो तर नेपालको माटो चाम्रो भएर हो कि गोरु थाकी हाल्छन ।</t>
+  </si>
+  <si>
+    <t>939493384040996864</t>
+  </si>
+  <si>
+    <t>939647137524019200</t>
+  </si>
+  <si>
+    <t>@bbcnepali tq</t>
+  </si>
+  <si>
+    <t>939494415852118021</t>
+  </si>
+  <si>
+    <t>@bbcnepali अब जस्तो नतिजा आएनी जनताले चित्त बुझाउनु पर्छ। जितेका नेताहरु नआतिकन देश बिकासमा लाग्नु पर्छ।</t>
+  </si>
+  <si>
+    <t>939533504093868033</t>
+  </si>
+  <si>
+    <t>@bbcnepali @BhagirathYogi सही कुरा! कसले सुरू गने अब? !</t>
+  </si>
+  <si>
+    <t>939525451260747776</t>
+  </si>
+  <si>
+    <t>@bbcnepali गगन थापाको विश्लेषण सहि छ।</t>
+  </si>
+  <si>
+    <t>939518505870794752</t>
+  </si>
+  <si>
+    <t>@bbcnepali @ruru_krishna @thapagk जस्ताले नै ज़िम्मा लिनु पर्ने कुरा भएकोले हाम्ले यस्मा थप्नुपर्ने केही भएन, शुभकामना बाहेक।</t>
+  </si>
+  <si>
+    <t>939511186856353794</t>
+  </si>
+  <si>
+    <t>939507148530204672</t>
+  </si>
+  <si>
+    <t>@bbcnepali मेरोपनि माग युवा लाई अगाडी बढाऔ, सभापतिले तत्काल राजीनाम गर्नुपर्यो</t>
+  </si>
+  <si>
+    <t>939504644576894976</t>
+  </si>
+  <si>
+    <t>@bbcnepali आफ्नो मलामी आफै कोही पनि गएको देखेको थिएनौं तर काङ्ग्रेस त्यसको अपवाद  बन्दियो। परै बाट भए पनि शुभकामना सुध्रियोस् काङ्ग्रेस ।</t>
+  </si>
+  <si>
+    <t>939496528141418496</t>
+  </si>
+  <si>
+    <t>@bbcnepali एकदम ठिक भन्नुभो गगन सर, अहिलेको परिणामले तेहिप्रमाणित गरिदियेको छ ! अब देश चलाउने पालो युवा पुस्ताकै हो !  अब आयेन्दा कुनै पनि नेताले सधै मैलेनै जित्छु युवालाई दिन्न भन्नू ठुलो मुर्खता हो र एस्तै बेइज्जती भयेर हार स्वीकार गर्न बाध्य हुनुपर्नेछ है होसियार !</t>
+  </si>
+  <si>
+    <t>939493970782113792</t>
+  </si>
+  <si>
+    <t>@bbcnepali भ्रम फैलाउने आफ्नै पार्टी। अरु पार्टीलाई दोष। युवा पुस्तामा एउटा राष्ट्रिय नेता छैनन् पुराना हटाउने हल्ला। यत्रो हार बाट पनि नसकिने भए। #नेपाल #Nepal</t>
+  </si>
+  <si>
+    <t>939490833090220032</t>
+  </si>
+  <si>
+    <t>@bbcnepali त्यो त हो तैपनि मैले बुझेअनुसार राजनीतिमा एकनासले टिक्न अनी सफल हुन त्यती छिटो सम्भव छैन।सवैलाई समय लाग्छ तर समय कुर्न कोही तयार छैनन् ,सबैलाई तुरुन्तै पद चाहिएको छ।प्रतिक्षा गर्दै,बुझ्दै,जनभावनाअनुसारको नीति लिँँदै अघि बढ्दा राम्रो होला।</t>
+  </si>
+  <si>
+    <t>939488759594266625</t>
+  </si>
+  <si>
+    <t>@bbcnepali राम्रो र सहि बिचार गगन जी को  ।</t>
+  </si>
+  <si>
+    <t>939476370043887616</t>
+  </si>
+  <si>
+    <t>939496217276321794</t>
+  </si>
+  <si>
+    <t>@bbcnepali लालबाबुलाई चिन्नु भो कोइराला ज्यु ?</t>
+  </si>
+  <si>
+    <t>939483404348874754</t>
+  </si>
+  <si>
+    <t>@bbcnepali उहा सच्चा र राम्रो नेता हुनुहुन्छ। चुनाबमा हार जित हुन्छ। फिक्कर नगर्नुस जनताको साथ छ यत्रो २ र ३ नम्बर पार्टी सँग चुनाब लड्नु नै काङ्ग्रेसको महन्ता हो। जित चाही काङ्ग्रेस को हो जस्ले जनताको अभिमत ले मात्रै सत्ता पाइन्छ भन्यो उसैको जित हो</t>
+  </si>
+  <si>
+    <t>939478060314873856</t>
+  </si>
+  <si>
+    <t>@bbcnepali शेखर कोइराला को कुरा सोही हो नेपाली जनताले नेपाल मा इस्थाइ सरकार चाहेका थिए र वाम गठ्बन्द्ले तेहि कुरा जन्ता सामु लागे र तेसाको रिजल्ट राम्रो आहेको छ</t>
+  </si>
+  <si>
+    <t>939408922632433664</t>
+  </si>
+  <si>
+    <t>939437391424524288</t>
+  </si>
+  <si>
+    <t>@bbcnepali हो बुडा हो</t>
+  </si>
+  <si>
+    <t>939421471826329600</t>
+  </si>
+  <si>
+    <t>@bbcnepali नेकपा एमालेका कम खर्चमा जित्ने नेतालाई कार्यकालको शुभकामना ।</t>
+  </si>
+  <si>
+    <t>939385099967221760</t>
+  </si>
+  <si>
+    <t>939425421078118400</t>
+  </si>
+  <si>
+    <t>@bbcnepali पाठ सीक्ला जस्तो छैन, सुँगूरलाई स्वर्ग जान्छस् भन्दा गुहु खान पाईन्छ र भन्थ्यो अरे</t>
+  </si>
+  <si>
+    <t>939421810088607745</t>
+  </si>
+  <si>
+    <t>939408698375417856</t>
+  </si>
+  <si>
+    <t>@bbcnepali यो पाठ सिक्ने पार्टी नै होइन।</t>
+  </si>
+  <si>
+    <t>939393324904980480</t>
+  </si>
+  <si>
+    <t>939385749459181569</t>
+  </si>
+  <si>
+    <t>@bbcnepali पाठ न सिके अर्कों exam मा नी फ़ेल हूंछ नी ।</t>
+  </si>
+  <si>
+    <t>939379249852698624</t>
+  </si>
+  <si>
+    <t>939436918516748288</t>
+  </si>
+  <si>
+    <t>@bbcnepali @BhagirathYogi कार्यकर्तालाई आग्रह गर्नुभन्दा बरु नेताहरु आफैँले कुनै पुर्वाग्रह नराखी आ-आफ्नो भुमीकाको समीक्षा गरे बेस होला, जनता/ कार्यकर्ता त नेता भन्दा धेरै बुझकी छन्।</t>
+  </si>
+  <si>
+    <t>939434145217896448</t>
+  </si>
+  <si>
+    <t>939401581199482880</t>
+  </si>
+  <si>
+    <t>939151383000961024</t>
+  </si>
+  <si>
+    <t>939153903316213760</t>
+  </si>
+  <si>
+    <t>@bbcnepali मलाई पैसाले चुनाब जितिन्छ जस्तो लाग्दैन, चुनाब जित्न सक्षम ब्यक्तित्व र रास्ट्रीय मुद्दा सही हुनु पर्छ ।</t>
+  </si>
+  <si>
+    <t>939148165508366336</t>
+  </si>
+  <si>
+    <t>939171614498762753</t>
+  </si>
+  <si>
+    <t>@bbcnepali संविधान बन्दा नुनतेल रोक्ने भारत अनि बाम अग्रता देखिदा रातारात पेट्रोलियम पदार्थको मुल्य वृद्धिको समाचार, केही शङ्का गर्न मिल्ला?</t>
+  </si>
+  <si>
+    <t>@bbcnepali केन्द्रमा प्रमुख दलको बहुमतको ५ बर्षको स्थिर सरकार,मधेशमा मधेश केन्द्रित दलको एकलौटि सरकार, कुनै खास खास क्षेत्रबाट नया शक्ति र विवेकशिल साझाको राष्ट्रिय दलको रुपमा सशक्त उपस्थिति/ बस् यहि हो यसपटकको चाहना/ अनि मात्र परिक्षण हुनेछ सबैको कुरा र काम बिचको भिन्नता र अन्तर</t>
+  </si>
+  <si>
+    <t>938807996473380864</t>
+  </si>
+  <si>
+    <t>939100904963403776</t>
+  </si>
+  <si>
+    <t>938810448006098945</t>
+  </si>
+  <si>
+    <t>@bbcnepali कतिपय बिश्‍लेषकले त नेपालको चुनावमा छिमेकीको हारजीत हुन्छ पनि भन्छन् । जातीय र क्षेत्रीय द्वेष फैलाउनेहरूलाई निरर्थक गर्न सके र कर्मचारीहरूमा नीहित सत्ता निर्वाचितहरुमा जान सके जोखिमहरू हराउदै जान्छन् ।</t>
+  </si>
+  <si>
+    <t>938797254844014592</t>
+  </si>
+  <si>
+    <t>939100709248815104</t>
+  </si>
+  <si>
+    <t>938782234638766088</t>
+  </si>
+  <si>
+    <t>938793897685217281</t>
+  </si>
+  <si>
+    <t>@bbcnepali देशले निकास पाउला भन्ने आशले डाका हरु लाई नचांहदा चांहदै भोट हालियो र हान्न लगाइयो अब हेरौं बिकास र समृद्धि को दिशामा लगछन कि खाल्टोमा लग्छन हेर्न बाँकि छ।</t>
+  </si>
+  <si>
+    <t>938744578403917824</t>
+  </si>
+  <si>
+    <t>938752352290406400</t>
+  </si>
+  <si>
+    <t>@bbcnepali विदेश मा नि यस्तो हुन्छ</t>
+  </si>
+  <si>
+    <t>938650874762678272</t>
+  </si>
+  <si>
+    <t>938665707172020225</t>
+  </si>
+  <si>
+    <t>@bbcnepali मतदानबाट व्यक्तिगत र पार्टीगत स्वार्थ भन्दा माथि उठेर सदैव देशको भलो चाहना नेता छानीउन् शुभकामना ।</t>
+  </si>
+  <si>
+    <t>938660866345418753</t>
+  </si>
+  <si>
+    <t>@bbcnepali मतदानको लागी प्रयोग गरिएको व्यानर फोटो उपयुक्त लागेन ।</t>
+  </si>
+  <si>
+    <t>938602630875697152</t>
+  </si>
+  <si>
+    <t>938612760333733888</t>
+  </si>
+  <si>
+    <t>@bbcnepali काम चलाउछ सरकार चाहिदैन।।।</t>
+  </si>
+  <si>
+    <t>938610404586131456</t>
+  </si>
+  <si>
+    <t>@bbcnepali काम चलाऊ ले जीम्मेबारी बुझाई घर जाने हो। निर्णय गर्ने होईन।</t>
+  </si>
+  <si>
+    <t>938609971285102592</t>
+  </si>
+  <si>
+    <t>@bbcnepali काम चलाऊ ले किन तोक्ने प्रदेश प्रमूख?</t>
+  </si>
+  <si>
+    <t>938441720240459776</t>
+  </si>
+  <si>
+    <t>938579344783323136</t>
+  </si>
+  <si>
+    <t>@bbcnepali नेपाली चुनावको मौलिकता हराएर गएको अनुभुति भएको छ।मौन अबधिमा पनि गोली नचल्नु,बम नपड्किनु हाताहाति नहुनु पैसा नबाडिनु आदि।</t>
+  </si>
+  <si>
+    <t>938412496259514369</t>
+  </si>
+  <si>
+    <t>938420569946570752</t>
+  </si>
+  <si>
+    <t>@bbcnepali 2054 साल देखी संगै संघर्ष गरेको माओवादी कति टुक्रा भयो ? किन यती टुक्रा भयो?संभिधानमस्यौदाकार समितिको संयोजक भई संभिधान बनाएर बाबुराम किन बाहिरए आफैले त्यसलाइ जलाईदिए किन ? लगत्तै नाकाबंदी एक्काशी भयो फेरी आफैं कसरी खुल्यो ? अनि अब कस्तो क्रांति हो यो?कसले प्रस्ट बनाऊँने यो कुरा?</t>
+  </si>
+  <si>
+    <t>938379012371615745</t>
+  </si>
+  <si>
+    <t>938380479081750529</t>
+  </si>
+  <si>
+    <t>@bbcnepali मानब मानब बिच धर्म र आस्ताको बिचको द्वन्द मानवजातिकैलागि ठूलो कलंक हो जो बाबरी मस्जीत तोडेर भाजपाले सुरू गर्यो भारतमा!!!</t>
+  </si>
+  <si>
+    <t>938299089225166851</t>
+  </si>
+  <si>
+    <t>938338102799581184</t>
+  </si>
+  <si>
+    <t>938248058143477760</t>
+  </si>
+  <si>
+    <t>938251664976330752</t>
+  </si>
+  <si>
+    <t>@bbcnepali सामुदायिक र सार्वजनिक विद्यालय चलाउन र तिनलाई सबल बनाउन राज्यको बीस प्रतिशत हाराहारीको बजेट कहाँ चुहिँदैछ र यही रकमबाट तलब भत्ता खानेहरू ती विद्यालय सञ्चालनको जिम्मेवारीबाट पन्छिँदै किन विदेशी प्रोजेक्टका परामर्शदाता बन्दैछन् भन्ने खबर पो लेख्नुपर्यो।</t>
+  </si>
+  <si>
+    <t>938245774978224134</t>
+  </si>
+  <si>
+    <t>938360364260982784</t>
+  </si>
+  <si>
+    <t>@bbcnepali बम बिस्फोटमा बारुदको संलग्नता सरकारद्वारा  पुष्टि #यस्तो समाचार सुन्न नपरोस् ।"</t>
+  </si>
+  <si>
+    <t>938335749799399425</t>
+  </si>
+  <si>
+    <t>938269351064485888</t>
+  </si>
+  <si>
+    <t>@bbcnepali आचार संहितामा नभयेको कुरालाई आचार संहिता विपरीत भयेको भनि चलेको गोलीलाई वैधता प्रदान गर्ने निर्णय गरेकै छ नि।</t>
+  </si>
+  <si>
+    <t>938250196466540544</t>
+  </si>
+  <si>
+    <t>@bbcnepali कारबाही गर्ने हैसियत र क्षमता पनि राख्नुपर्यो। निवार्चन आयोग स्वतन्त्र संवैधानिक निकाय नभएर उहिल्यै सरकारको विनाविभागीय मन्त्रालय भइसकेपछि यो के खबर भयो र।</t>
+  </si>
+  <si>
+    <t>938090557544521728</t>
+  </si>
+  <si>
+    <t>938235474103058433</t>
+  </si>
+  <si>
+    <t>@bbcnepali मतदान मात्र होइन गाउँ बिकास को लागि पनि फर्कनु पर्यो जनता हरु।</t>
+  </si>
+  <si>
+    <t>938207024743006208</t>
+  </si>
+  <si>
+    <t>optimistic</t>
+  </si>
+  <si>
+    <t>@bbcnepali के यो सहि तरीका होला??</t>
+  </si>
+  <si>
+    <t>happy</t>
+  </si>
+  <si>
+    <t>@bbcnepali घमण्डले आफैलाई खान्छ भन्ने सहि हो...👏👏</t>
+  </si>
+  <si>
+    <t>@bbcnepali देशको  भविष्यको सवाल छ। भोट त हाल्नै पर्यो नि। होइन  त??</t>
+  </si>
+  <si>
+    <t>@bbcnepali सर्व साधारण र गरिब नागरिकले उलङ्घन गरे पो कार्वाही । धनी र नेताले उलङ्घन  गरे कार्वाही  नहुने नेपाली चलनकै उदाहरण होला यो पनि । ,सानालाई ऐन ठूलालाई चैन भनेको यहि हो ।</t>
+  </si>
+  <si>
+    <t>@bbcnepali @ManaviPaudel @RabindraMishra @SuryaRAcharya जेजती मत पाउनु भएको छ। सम्मानजनक छ। नेतृत्वमा जानकैलागी होईन , राष्ट्रको समृद्धिकोलागी लागौं । अवसरहरु प्रशस्त छन्</t>
+  </si>
+  <si>
+    <t>@bbcnepali बामगठबन्धनले हार भए जनताको मतलाई स्विकार्न गाह्रो हुनेथियो तर लोकतान्त्रीक बिचार लिएका हरु सजिलै स्विकार्छन</t>
+  </si>
+  <si>
+    <t>@bbcnepali अब मतदान अधिकृतको दस्तखत नमिलेर मतपत्र बाउन्स हुने भयो , एउटा केन्द्र मा  ३ हजार दस्तखत गर्दा मतदान अधिकृतले कति मिलाउन सक्छन ? किचलो झिक्न अरू विषय नपाए जस्तो लाग्यो ।</t>
+  </si>
+  <si>
+    <t>negative</t>
+  </si>
+  <si>
+    <t>@bbcnepali देश कुन बाटोमा हिडाउने भन्ने तय गर्ने एउटा मुख्य आधार निर्वाचन पनि हो। त्यसैले भोलि देश विकास र सम्बृद्दिको बाटोमा अगाडि बढेन भनी पुर्पुरो ठोक्नु भन्दा हाम्रा होईन राम्रालाई भोट दियर पठाउँ ।तपाई र मेरो एक/एक भोट नै हाम्रो भविष्यका लागि निर्णायक बन्नेछ।</t>
+  </si>
+  <si>
+    <t>@bbcnepali चाडै महाधिवेशन गरि सभापतिमा अर्को व्यक्ति आएमा शायद केही सुधार होला, नत्र ओरालो लाग्नु बाहेक ने. का. ले अब माखो मार्ने वाला छैन ।</t>
+  </si>
+  <si>
+    <t>sad</t>
+  </si>
+  <si>
+    <t>disappointed</t>
+  </si>
+  <si>
+    <t>pessimistic</t>
+  </si>
+  <si>
+    <t>excited</t>
+  </si>
+  <si>
+    <t>neutral</t>
+  </si>
+  <si>
+    <t>thankful</t>
+  </si>
+  <si>
+    <t>positive</t>
   </si>
 </sst>
 </file>
@@ -132,16 +640,27 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -160,6 +679,10 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="bbcnepali_1" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="bbcnepali" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
@@ -450,128 +973,1043 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D82"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="19.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="88.7109375" style="3" customWidth="1"/>
+    <col min="1" max="2" width="19.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="81.140625" style="1" customWidth="1"/>
     <col min="4" max="4" width="96" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="5"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="4" t="s">
         <v>4</v>
       </c>
+      <c r="D2" s="5"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="4" t="s">
         <v>15</v>
       </c>
+      <c r="D3" s="5"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="4" t="s">
         <v>16</v>
       </c>
+      <c r="D4" s="5"/>
     </row>
     <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="4" t="s">
         <v>20</v>
       </c>
+      <c r="D5" s="5"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="4" t="s">
         <v>19</v>
       </c>
+      <c r="D6" s="5"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="1"/>
+      <c r="D7" s="6"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="4" t="s">
         <v>12</v>
       </c>
+      <c r="D8" s="5"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="4" t="s">
         <v>17</v>
       </c>
+      <c r="D9" s="5" t="s">
+        <v>178</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="4">
+      <c r="A10" s="3">
         <v>9.3952432157539098E+17</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B10" s="3">
         <v>9.3963492418472704E+17</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="7" t="s">
         <v>21</v>
+      </c>
+      <c r="D10" s="5"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="5"/>
+    </row>
+    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" s="5"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" s="5"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" s="5"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15" s="5"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D19" s="5"/>
+    </row>
+    <row r="20" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D22" s="5"/>
+    </row>
+    <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A24" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D24" s="5"/>
+    </row>
+    <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A27" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D27" s="5"/>
+    </row>
+    <row r="28" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D28" s="5"/>
+    </row>
+    <row r="29" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A29" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D29" s="5"/>
+    </row>
+    <row r="30" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D30" s="5"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D31" s="5"/>
+    </row>
+    <row r="32" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A32" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D32" s="5"/>
+    </row>
+    <row r="33" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A33" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D33" s="5"/>
+    </row>
+    <row r="34" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D34" s="5"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D35" s="5"/>
+    </row>
+    <row r="36" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A36" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D36" s="5"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D37" s="5"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B38" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D38" s="5"/>
+    </row>
+    <row r="39" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A39" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B39" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D39" s="5"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B40" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="D40" s="5"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B41" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D41" s="5"/>
+    </row>
+    <row r="42" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A42" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B42" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D42" s="5"/>
+    </row>
+    <row r="43" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A43" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B43" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="D43" s="5"/>
+    </row>
+    <row r="44" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A44" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B44" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D44" s="5"/>
+    </row>
+    <row r="45" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A45" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B45" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D45" s="5"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B46" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="B47" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="D47" s="5"/>
+    </row>
+    <row r="48" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A48" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="B48" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="D48" s="5"/>
+    </row>
+    <row r="49" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A49" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="B49" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="D49" s="5" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="B50" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="D50" s="5" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="B51" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="D51" s="5" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="B52" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="D52" s="5" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="B53" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="D53" s="5" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="B54" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="D54" s="5" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A55" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="B55" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="D55" s="5"/>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="B56" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="D56" s="5" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A57" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="B57" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="D57" s="5"/>
+    </row>
+    <row r="58" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A58" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="B58" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="D58" s="5"/>
+    </row>
+    <row r="59" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A59" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="B59" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="C59" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="D59" s="5"/>
+    </row>
+    <row r="60" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A60" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="B60" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="C60" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="D60" s="5"/>
+    </row>
+    <row r="61" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A61" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="B61" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="C61" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="D61" s="5"/>
+    </row>
+    <row r="62" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A62" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="B62" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="C62" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="D62" s="5"/>
+    </row>
+    <row r="63" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A63" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="B63" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="C63" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="D63" s="5"/>
+    </row>
+    <row r="64" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A64" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="B64" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="C64" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="D64" s="5"/>
+    </row>
+    <row r="65" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A65" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="B65" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="C65" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="D65" s="5" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="B66" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="C66" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="D66" s="5" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A67" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="B67" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="C67" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="D67" s="5"/>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="B68" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="C68" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="D68" s="5"/>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="B69" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="C69" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="D69" s="5"/>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="B70" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="C70" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="D70" s="5"/>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="B71" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="C71" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="D71" s="5"/>
+    </row>
+    <row r="72" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A72" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="B72" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="C72" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="D72" s="5"/>
+    </row>
+    <row r="73" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A73" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="B73" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="C73" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="D73" s="5"/>
+    </row>
+    <row r="74" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A74" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="B74" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="C74" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="D74" s="5"/>
+    </row>
+    <row r="75" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A75" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="B75" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="C75" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="D75" s="5"/>
+    </row>
+    <row r="76" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A76" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="B76" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="C76" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="D76" s="5"/>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="B77" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="C77" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="D77" s="5"/>
+    </row>
+    <row r="78" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A78" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="B78" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="C78" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="D78" s="5"/>
+    </row>
+    <row r="79" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A79" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="B79" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="C79" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="D79" s="5"/>
+    </row>
+    <row r="80" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A80" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="B80" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="C80" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="D80" s="5"/>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="B81" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="C81" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="D81" s="5" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="B82" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="C82" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="D82" s="5" t="s">
+        <v>169</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added data and analyzer code.
</commit_message>
<xml_diff>
--- a/data/dataset.xlsx
+++ b/data/dataset.xlsx
@@ -7,11 +7,12 @@
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Dateset" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="bbcnepali" localSheetId="0">Sheet1!$A$1:$C$9</definedName>
-    <definedName name="bbcnepali_1" localSheetId="0">Sheet1!$A$11:$C$82</definedName>
+    <definedName name="bbcnepali" localSheetId="0">Dateset!$A$2:$C$10</definedName>
+    <definedName name="bbcnepali_1" localSheetId="0">Dateset!$A$11:$C$79</definedName>
+    <definedName name="NepalPoliceHQ" localSheetId="0">Dateset!$A$80:$C$88</definedName>
   </definedNames>
   <calcPr calcId="122211"/>
 </workbook>
@@ -37,11 +38,20 @@
       </textFields>
     </textPr>
   </connection>
+  <connection id="3" name="NepalPoliceHQ" type="6" refreshedVersion="5" background="1" saveData="1">
+    <textPr codePage="65001" sourceFile="E:\Projects\SentimentAnalysis\SentimentAnalysis\data\NepalPoliceHQ.csv" tab="0" comma="1">
+      <textFields count="3">
+        <textField type="text"/>
+        <textField type="text"/>
+        <textField type="text"/>
+      </textFields>
+    </textPr>
+  </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="217">
   <si>
     <t>939524321575391233</t>
   </si>
@@ -136,9 +146,6 @@
     <t>939528412246536193</t>
   </si>
   <si>
-    <t>@bbcnepali यी curd bittenricey जे पनि बोल्छन् भन्ने हाम्लाइ लागि राच</t>
-  </si>
-  <si>
     <t>939526985813856257</t>
   </si>
   <si>
@@ -175,9 +182,6 @@
     <t>939510428643684353</t>
   </si>
   <si>
-    <t>@bbcnepali चलखेल...... lol</t>
-  </si>
-  <si>
     <t>939509252422545409</t>
   </si>
   <si>
@@ -205,18 +209,12 @@
     <t>939504017146757122</t>
   </si>
   <si>
-    <t>@bbcnepali 😂😂</t>
-  </si>
-  <si>
     <t>939499929235542017</t>
   </si>
   <si>
     <t>939522624622796800</t>
   </si>
   <si>
-    <t>@bbcnepali जनताले विश्वास गरेर नपुग्ने ।अरू कसले विश्वास गर्नुपर्ने हाे।नेपाली कांग्रेस संग मिलेर  एमाले र माअाेवादीले सरकार चलाई सकेकाे हाेईन र। अनि  माअाेवादी र एमाले मिलेर पनि सरकार चलायकै हाे।अधिनायकवाद अाउनेभए त पहिलेनै अाईसकेकाे हुन्थ्यो ।</t>
-  </si>
-  <si>
     <t>939505773268295680</t>
   </si>
   <si>
@@ -235,9 +233,6 @@
     <t>939647137524019200</t>
   </si>
   <si>
-    <t>@bbcnepali tq</t>
-  </si>
-  <si>
     <t>939494415852118021</t>
   </si>
   <si>
@@ -292,9 +287,6 @@
     <t>939490833090220032</t>
   </si>
   <si>
-    <t>@bbcnepali त्यो त हो तैपनि मैले बुझेअनुसार राजनीतिमा एकनासले टिक्न अनी सफल हुन त्यती छिटो सम्भव छैन।सवैलाई समय लाग्छ तर समय कुर्न कोही तयार छैनन् ,सबैलाई तुरुन्तै पद चाहिएको छ।प्रतिक्षा गर्दै,बुझ्दै,जनभावनाअनुसारको नीति लिँँदै अघि बढ्दा राम्रो होला।</t>
-  </si>
-  <si>
     <t>939488759594266625</t>
   </si>
   <si>
@@ -520,9 +512,6 @@
     <t>938360364260982784</t>
   </si>
   <si>
-    <t>@bbcnepali बम बिस्फोटमा बारुदको संलग्नता सरकारद्वारा  पुष्टि #यस्तो समाचार सुन्न नपरोस् ।"</t>
-  </si>
-  <si>
     <t>938335749799399425</t>
   </si>
   <si>
@@ -589,9 +578,6 @@
     <t>sad</t>
   </si>
   <si>
-    <t>disappointed</t>
-  </si>
-  <si>
     <t>pessimistic</t>
   </si>
   <si>
@@ -605,13 +591,124 @@
   </si>
   <si>
     <t>positive</t>
+  </si>
+  <si>
+    <t>939130458553532416</t>
+  </si>
+  <si>
+    <t>939387326362296320</t>
+  </si>
+  <si>
+    <t>938357091432931333</t>
+  </si>
+  <si>
+    <t>938511176492707841</t>
+  </si>
+  <si>
+    <t>@NepalPoliceHQ साइकल सवारी साधनमा पर्छ की पर्दैन होला, महोदय ?</t>
+  </si>
+  <si>
+    <t>938399396361748481</t>
+  </si>
+  <si>
+    <t>@NepalPoliceHQ @dahalshivaji नेपाल बन्द नै भनेर घोषणा गर्दा हुन्छ त किन सार्वजनिक बिदा भनिराख्नु!</t>
+  </si>
+  <si>
+    <t>938359659995439104</t>
+  </si>
+  <si>
+    <t>937566294609600512</t>
+  </si>
+  <si>
+    <t>937566845573390336</t>
+  </si>
+  <si>
+    <t>936571761155387392</t>
+  </si>
+  <si>
+    <t>936869371015708672</t>
+  </si>
+  <si>
+    <t>@NepalPoliceHQ किन त सेरे दाइले थापाए भनी गाली गर्नु हुन्न र ?</t>
+  </si>
+  <si>
+    <t>936635424579055616</t>
+  </si>
+  <si>
+    <t>936606223368994818</t>
+  </si>
+  <si>
+    <t>@NepalPoliceHQ ठोक्दे हुन्छ गोली</t>
+  </si>
+  <si>
+    <t>936558449302876165</t>
+  </si>
+  <si>
+    <t>936871176038526976</t>
+  </si>
+  <si>
+    <t>@NepalPoliceHQ डाक्टर बोलाएर अपरेसन गरिदेउ !! जस्को सुसु गर्न मात्र काम लागोस !</t>
+  </si>
+  <si>
+    <t>@NepalPoliceHQ मैले त कसम कुकुर बम देखेको, धन्न।</t>
+  </si>
+  <si>
+    <t>@NepalPoliceHQ ६ मिनेट अघी म‌ १२ बजे कसरी  पुग्नु काठमाण्डौँ</t>
+  </si>
+  <si>
+    <t>@NepalPoliceHQ राजा मार्ने पक्राउ परेन... घुस लिने पुलिस पक्रउ परेन... सलाम ठोक्नुस नेता हरूको अरु के काम छ र नेपाल पुलिस को</t>
+  </si>
+  <si>
+    <t>upset</t>
+  </si>
+  <si>
+    <t>displeased</t>
+  </si>
+  <si>
+    <t>sarcastic</t>
+  </si>
+  <si>
+    <t>@bbcnepali जनताले विश्वास गरेर नपुग्ने ।अरू कसले विश्वास गर्नुपर्ने हो।नेपाली कांग्रेस संग मिलेर  एमाले र माओवादीले सरकार चलाई सकेको होईन र। अनि  माओवादी र एमाले मिलेर पनि सरकार चलायकै हो।अधिनायकवाद आउनेभए त पहिलेनै आईसकेको हुन्थ्यो ।</t>
+  </si>
+  <si>
+    <t>@bbcnepali त्यो त हो तैपनि मैले बुझेअनुसार राजनीतिमा एकनासले टिक्न अनी सफल हुन त्यती छिटो सम्भव छैन।सवैलाई समय लाग्छ तर समय कुर्न कोही तयार छैनन् ,सबैलाई तुरुन्तै पद चाहिएको छ।प्रतिक्षा गर्दै,बुझ्दै,जनभावनाअनुसारको नीति लिँदै अघि बढ्दा राम्रो होला।</t>
+  </si>
+  <si>
+    <t>@bbcnepali चलखेल...... हाहा</t>
+  </si>
+  <si>
+    <t>@bbcnepali धन्यवाद</t>
+  </si>
+  <si>
+    <t>@bbcnepali हाहा</t>
+  </si>
+  <si>
+    <t>@NepalPoliceHQ फेसबुक र ट्वीट मा आउने हिंसक बिचार लाई कसरी रोकने हो बिचार पुरयाइयोस्।</t>
+  </si>
+  <si>
+    <t>@bbcnepali बम बिस्फोटमा बारुदको संलग्नता सरकारद्वारा  पुष्टि यस्तो समाचार सुन्न नपरोस् ।</t>
+  </si>
+  <si>
+    <t>@bbcnepali यी दहि चिऊरा जे पनि बोल्छन् भन्ने हाम्लाइ लागि राच</t>
+  </si>
+  <si>
+    <t>reply_id</t>
+  </si>
+  <si>
+    <t>tweet_id</t>
+  </si>
+  <si>
+    <t>full_text</t>
+  </si>
+  <si>
+    <t>label</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -619,13 +716,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -640,7 +751,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -658,9 +769,15 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -679,10 +796,14 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="NepalPoliceHQ" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="bbcnepali_1" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="bbcnepali" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
@@ -973,140 +1094,158 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D82"/>
+  <dimension ref="A1:D88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="D59" sqref="D59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="19.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="81.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="96" customWidth="1"/>
+    <col min="3" max="3" width="61.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="5"/>
+    <row r="1" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>214</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>213</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>215</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>216</v>
+      </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="5"/>
+        <v>2</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>162</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="5"/>
+        <v>4</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>203</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="5"/>
-    </row>
-    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" s="5"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="5"/>
+        <v>20</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>203</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" s="6"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" s="5"/>
+        <v>18</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>203</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B10" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C10" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="5" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="3">
-        <v>9.3952432157539098E+17</v>
-      </c>
-      <c r="B10" s="3">
-        <v>9.3963492418472704E+17</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D10" s="5"/>
+      <c r="D10" s="5" t="s">
+        <v>171</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
@@ -1118,7 +1257,9 @@
       <c r="C11" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D11" s="5"/>
+      <c r="D11" s="5" t="s">
+        <v>204</v>
+      </c>
     </row>
     <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
@@ -1130,7 +1271,9 @@
       <c r="C12" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="5"/>
+      <c r="D12" s="5" t="s">
+        <v>177</v>
+      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
@@ -1142,7 +1285,9 @@
       <c r="C13" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D13" s="5"/>
+      <c r="D13" s="5" t="s">
+        <v>178</v>
+      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
@@ -1154,301 +1299,333 @@
       <c r="C14" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D14" s="5"/>
+      <c r="D14" s="5" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D15" s="5"/>
+        <v>212</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>171</v>
+      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>3</v>
+        <v>31</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>15</v>
+        <v>168</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>185</v>
+        <v>162</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="D18" s="5" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D19" s="5"/>
-    </row>
-    <row r="20" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C20" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D20" s="5" t="s">
         <v>175</v>
       </c>
-      <c r="D20" s="5" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>12</v>
+        <v>39</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="D22" s="5"/>
-    </row>
-    <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>38</v>
+        <v>207</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D24" s="5"/>
-    </row>
-    <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="D27" s="5"/>
-    </row>
-    <row r="28" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="D28" s="5"/>
+        <v>209</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="29" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
-        <v>6</v>
+        <v>52</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="D29" s="5"/>
-    </row>
-    <row r="30" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>205</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
-        <v>6</v>
+        <v>52</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="C30" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A31" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D30" s="5"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="6" t="s">
-        <v>6</v>
-      </c>
       <c r="B31" s="6" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="D31" s="5"/>
-    </row>
-    <row r="32" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="D32" s="5"/>
-    </row>
-    <row r="33" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+        <v>208</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="D33" s="5"/>
-    </row>
-    <row r="34" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
-        <v>55</v>
+        <v>13</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="D34" s="5"/>
+        <v>63</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
-        <v>62</v>
+        <v>13</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="D35" s="5"/>
+        <v>65</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="36" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
-        <v>62</v>
+        <v>13</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="D36" s="5"/>
+        <v>67</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
         <v>13</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="D37" s="5"/>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+        <v>163</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
         <v>13</v>
       </c>
@@ -1458,9 +1635,11 @@
       <c r="C38" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="D38" s="5"/>
-    </row>
-    <row r="39" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="D38" s="5" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
         <v>13</v>
       </c>
@@ -1470,9 +1649,11 @@
       <c r="C39" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="D39" s="5"/>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D39" s="5" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
         <v>13</v>
       </c>
@@ -1480,35 +1661,41 @@
         <v>73</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>170</v>
-      </c>
-      <c r="D40" s="5"/>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
         <v>13</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="D41" s="5"/>
-    </row>
-    <row r="42" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
         <v>13</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="D42" s="5"/>
-    </row>
-    <row r="43" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+        <v>206</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="6" t="s">
         <v>13</v>
       </c>
@@ -1518,101 +1705,111 @@
       <c r="C43" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="D43" s="5"/>
-    </row>
-    <row r="44" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="D43" s="5" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
-        <v>13</v>
+        <v>80</v>
       </c>
       <c r="B44" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D44" s="5" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A45" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="C44" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="D44" s="5"/>
-    </row>
-    <row r="45" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A45" s="6" t="s">
-        <v>13</v>
-      </c>
       <c r="B45" s="6" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="D45" s="5"/>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+      <c r="D45" s="5" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
-        <v>13</v>
+        <v>80</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="6" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B47" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D47" s="5" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A48" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="C47" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="D47" s="5"/>
-    </row>
-    <row r="48" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A48" s="6" t="s">
-        <v>86</v>
-      </c>
       <c r="B48" s="6" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="D48" s="5"/>
+        <v>91</v>
+      </c>
+      <c r="D48" s="5" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="49" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="6" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>187</v>
+        <v>175</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>95</v>
+        <v>165</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B51" s="6" t="s">
         <v>96</v>
@@ -1621,40 +1818,40 @@
         <v>97</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A52" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="B52" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="B52" s="6" t="s">
-        <v>99</v>
-      </c>
       <c r="C52" s="4" t="s">
-        <v>100</v>
+        <v>173</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="6" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="B53" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="D53" s="5" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A54" s="6" t="s">
         <v>101</v>
-      </c>
-      <c r="C53" s="4" t="s">
-        <v>172</v>
-      </c>
-      <c r="D53" s="5" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="6" t="s">
-        <v>98</v>
       </c>
       <c r="B54" s="6" t="s">
         <v>102</v>
@@ -1663,96 +1860,108 @@
         <v>103</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" s="6" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="B55" s="6" t="s">
         <v>104</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="D55" s="5"/>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+        <v>169</v>
+      </c>
+      <c r="D55" s="5" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A56" s="6" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="B56" s="6" t="s">
         <v>105</v>
       </c>
       <c r="C56" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="D56" s="5" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A57" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="D56" s="5" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A57" s="6" t="s">
+      <c r="B57" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="B57" s="6" t="s">
+      <c r="C57" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="C57" s="4" t="s">
+      <c r="D57" s="5" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A58" s="6" t="s">
         <v>109</v>
-      </c>
-      <c r="D57" s="5"/>
-    </row>
-    <row r="58" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A58" s="6" t="s">
-        <v>107</v>
       </c>
       <c r="B58" s="6" t="s">
         <v>110</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>176</v>
-      </c>
-      <c r="D58" s="5"/>
-    </row>
-    <row r="59" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+      <c r="D58" s="5" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A59" s="6" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="B59" s="6" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="C59" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="D59" s="5" t="s">
         <v>177</v>
       </c>
-      <c r="D59" s="5"/>
-    </row>
-    <row r="60" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="60" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A60" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="B60" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="C60" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="D60" s="5" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A61" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="B61" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="C61" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="B60" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="C60" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="D60" s="5"/>
-    </row>
-    <row r="61" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A61" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="B61" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="C61" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="D61" s="5"/>
-    </row>
-    <row r="62" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="D61" s="5" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A62" s="6" t="s">
         <v>119</v>
       </c>
@@ -1760,256 +1969,374 @@
         <v>120</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="D62" s="5"/>
-    </row>
-    <row r="63" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+      <c r="D62" s="5" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="6" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="B63" s="6" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="D63" s="5"/>
-    </row>
-    <row r="64" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+      <c r="D63" s="5" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A64" s="6" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B64" s="6" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="D64" s="5"/>
+        <v>127</v>
+      </c>
+      <c r="D64" s="5" t="s">
+        <v>162</v>
+      </c>
     </row>
     <row r="65" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A65" s="6" t="s">
         <v>125</v>
       </c>
       <c r="B65" s="6" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="D65" s="5" t="s">
-        <v>181</v>
+        <v>203</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="6" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B66" s="6" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="D66" s="5" t="s">
-        <v>185</v>
+        <v>171</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A67" s="6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B67" s="6" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="D67" s="5"/>
+        <v>134</v>
+      </c>
+      <c r="D67" s="5" t="s">
+        <v>171</v>
+      </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B68" s="6" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="D68" s="5"/>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+        <v>136</v>
+      </c>
+      <c r="D68" s="5" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A69" s="6" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B69" s="6" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="D69" s="5"/>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+      <c r="D69" s="5" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A70" s="6" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="B70" s="6" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="D70" s="5"/>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+      <c r="D70" s="5" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A71" s="6" t="s">
-        <v>136</v>
+        <v>143</v>
       </c>
       <c r="B71" s="6" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="D71" s="5"/>
-    </row>
-    <row r="72" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+      <c r="D71" s="5" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A72" s="6" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="B72" s="6" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="D72" s="5"/>
-    </row>
-    <row r="73" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+        <v>172</v>
+      </c>
+      <c r="D72" s="5" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A73" s="6" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="B73" s="6" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="D73" s="5"/>
+        <v>150</v>
+      </c>
+      <c r="D73" s="5" t="s">
+        <v>203</v>
+      </c>
     </row>
     <row r="74" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A74" s="6" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B74" s="6" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="D74" s="5"/>
+        <v>211</v>
+      </c>
+      <c r="D74" s="5" t="s">
+        <v>203</v>
+      </c>
     </row>
     <row r="75" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A75" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B75" s="6" t="s">
         <v>153</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>179</v>
-      </c>
-      <c r="D75" s="5"/>
-    </row>
-    <row r="76" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+        <v>167</v>
+      </c>
+      <c r="D75" s="5" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A76" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="B76" s="6" t="s">
         <v>154</v>
       </c>
-      <c r="B76" s="6" t="s">
+      <c r="C76" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="C76" s="4" t="s">
+      <c r="D76" s="5" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A77" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="B77" s="6" t="s">
         <v>156</v>
       </c>
-      <c r="D76" s="5"/>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="6" t="s">
+      <c r="C77" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="B77" s="6" t="s">
+      <c r="D77" s="5" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A78" s="6" t="s">
         <v>158</v>
       </c>
-      <c r="C77" s="4" t="s">
+      <c r="B78" s="6" t="s">
         <v>159</v>
       </c>
-      <c r="D77" s="5"/>
-    </row>
-    <row r="78" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A78" s="6" t="s">
-        <v>157</v>
-      </c>
-      <c r="B78" s="6" t="s">
+      <c r="C78" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="C78" s="4" t="s">
-        <v>174</v>
-      </c>
-      <c r="D78" s="5"/>
+      <c r="D78" s="5" t="s">
+        <v>176</v>
+      </c>
     </row>
     <row r="79" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A79" s="6" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B79" s="6" t="s">
         <v>161</v>
       </c>
       <c r="C79" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="D79" s="5" t="s">
         <v>162</v>
       </c>
-      <c r="D79" s="5"/>
     </row>
     <row r="80" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A80" s="6" t="s">
-        <v>157</v>
-      </c>
-      <c r="B80" s="6" t="s">
-        <v>163</v>
-      </c>
-      <c r="C80" s="4" t="s">
-        <v>164</v>
-      </c>
-      <c r="D80" s="5"/>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" s="6" t="s">
-        <v>165</v>
-      </c>
-      <c r="B81" s="6" t="s">
-        <v>166</v>
-      </c>
-      <c r="C81" s="4" t="s">
-        <v>167</v>
-      </c>
-      <c r="D81" s="5" t="s">
+      <c r="A80" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="B80" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="C80" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="D80" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A81" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="B81" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="C81" s="8" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" s="6" t="s">
-        <v>165</v>
-      </c>
-      <c r="B82" s="6" t="s">
-        <v>168</v>
-      </c>
-      <c r="C82" s="4" t="s">
-        <v>173</v>
+      <c r="D81" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A82" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="B82" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="C82" s="8" t="s">
+        <v>186</v>
       </c>
       <c r="D82" s="5" t="s">
-        <v>169</v>
+        <v>171</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="B83" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="C83" s="8" t="s">
+        <v>200</v>
+      </c>
+      <c r="D83" s="5" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="B84" s="8" t="s">
+        <v>189</v>
+      </c>
+      <c r="C84" s="8" t="s">
+        <v>199</v>
+      </c>
+      <c r="D84" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="B85" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="C85" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="D85" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A86" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="B86" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="C86" s="8" t="s">
+        <v>201</v>
+      </c>
+      <c r="D86" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="B87" s="8" t="s">
+        <v>194</v>
+      </c>
+      <c r="C87" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="D87" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A88" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="B88" s="8" t="s">
+        <v>197</v>
+      </c>
+      <c r="C88" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="D88" t="s">
+        <v>202</v>
       </c>
     </row>
   </sheetData>

</xml_diff>